<commit_message>
updated LBM measures artifacts
</commit_message>
<xml_diff>
--- a/StateOfPractice/DomainMeasurements/LBM-Peter/Completed_LBS_Combined_MeasurementTemplate_EmpiricalMeasures_ADDED_MUSUBI_UPDATED_STATS.xlsx
+++ b/StateOfPractice/DomainMeasurements/LBM-Peter/Completed_LBS_Combined_MeasurementTemplate_EmpiricalMeasures_ADDED_MUSUBI_UPDATED_STATS.xlsx
@@ -1472,49 +1472,49 @@
     <t xml:space="preserve">({yes*, no, unclear}) *list via string</t>
   </si>
   <si>
-    <t xml:space="preserve">yes, website, User Manual, license, README, mail shots, Example Simulations, training presentation, tutorial exercises, articles, philosophy and overview, development history and functionality, requirements, licensing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes, version control, README, CONTRIBUTING, AUTHORS, CHANGELOG, COPYING, Python interface documentation, website (doxygen, doanloads, publications, history, funding, data privacy, imprint, C++ documentation including tutorials, pystencils)</t>
+    <t xml:space="preserve">yes, website, User Manual, license, README, mail shots, Example Simulations, training presentation, tutorial exercises, articles, philosophy and overview, development history and functionality, requirements, licensing, citation (in user manual), acknowledgements (in user manual)), getting started (in user manual)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes, version control, README, CONTRIBUTING (only instructions for getting agreement), AUTHORS, CHANGELOG, COPYING, Python interface documentation, website (doxygen, doanloads, publications, history, funding, data privacy, imprint, C++ documentation including tutorials, pystencils), citation (in readme), getting started</t>
   </si>
   <si>
     <t xml:space="preserve">yes, sourceforge site (including wiki, CVS data, installation instructions, code, introduction, copying, authors), readme, todo, copying, authors </t>
   </si>
   <si>
-    <t xml:space="preserve">yes, website, version control, readme, bugs, to do, installation, internals, models, media, performance, api, about, tutorial, simulations, examples and test cases, release notes, media files, motivation and design principles, youtube, supported features and models, reference manual encompasses many of the prior sections</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes, website, version control, readme, contributing, change log, copying, doxyfile, publications, forum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes, website, user guide, news, overview, authors, partners and friends, showcases, articles, tech. Reports, developer guide, forum, FAQ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes, version control, README, COPYING (release notes), CHANGES, User Guide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes, version control, README,  authors, website (welcome, acknowledgments, examples, featured publications, download and installation, tutorials)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes, README, NOTICE, version control, wiki(about, key people, validation, performance, original publication, installation, testing, post-processor, licensing, release notes, for developers)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes, README, tutorial, contributing, changes, version control, website</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes, webpage, wiki</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes, README, authors, contributing, requirements, getting started  (part of README), credits (part of README), version control, usage, installation, modules</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes, README, version control, contributors, documentation, tutorial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes, README, Tutorial Notebooks, API Reference, version control, Project members</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes, manual, webpage</t>
+    <t xml:space="preserve">yes, website, version control, readme, bugs, to do, installation, internals, models, media, performance, api, about, tutorial, simulations, examples and test cases, release notes, media files, motivation and design principles, youtube, supported features and models, reference manual encompasses many of the prior sections, cite (in about doc), acknowledgements (in about doc), getting started</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes, website, version control, readme, contributing, change log, copying, doxyfile, publications, forum, citation (in readme), getting started (in manual)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes, website, user guide, news, overview, authors, partners and friends, showcases, articles, tech. Reports, developer guide, forum, FAQ, citation, getting started</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes, version control, README, COPYING (release notes), CHANGES, User Guide (has similar to getting started)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes, version control, README,  authors, website (welcome, acknowledgments, examples, featured publications, download and installation, tutorials), getting started</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes, README, NOTICE, version control, wiki(about, key people, validation, performance, original publication, installation, testing, post-processor, licensing, release notes, for developers), coding style, getting started</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes, README, tutorial, contributing, changes, version control, website, getting started</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes, webpage, wiki, getting started (quick start)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes, README, authors, contributing (2021), requirements, getting started  (part of README), credits (part of README), version control, usage, installation, modules, citation (in readme)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes, README, version control, contributors, documentation, tutorial, getting started</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes, README, Tutorial Notebooks, API Reference, version control, Project members, citation (in readme), getting started, contributing (added 2021)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes, manual (includes something similar to getting stared), webpage</t>
   </si>
   <si>
     <t xml:space="preserve">Yes, Manual, videos</t>
@@ -1526,22 +1526,22 @@
     <t xml:space="preserve">Yes, version control, README, job log</t>
   </si>
   <si>
-    <t xml:space="preserve">yes, Reference Manual, makefile, readme, authors, version control</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes, User’s Guide, makefile, readme, references, requirements, tutorials, version control, authors, release notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes,  Installation Guide, Tutorials, User Interface, Authors, FAQ, makefile, README, version control</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HemeLB documentation, Makefile, version control, README</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manual (aka notes), Student Guide (by request),  README, Makefile, version control</t>
-  </si>
-  <si>
-    <t xml:space="preserve">requirements, tutorials, test cases, makefile,
+    <t xml:space="preserve">yes, Reference Manual, makefile, readme, authors, version control, citation (in readme), getting started</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes, User’s Guide, makefile, readme, references, requirements, tutorials, version control, authors, release notes, contributing, citation (in readme), getting started</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes,  Installation Guide, Tutorials, User Interface, Authors, FAQ, makefile, README, version control, contributing (in wiki), roadmap (in wiki)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HemeLB documentation, Makefile, version control, README, coding guide (in wiki)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manual (aka notes), Student Guide (by request),  README, Makefile, version control, citation (in readme), getting started</t>
+  </si>
+  <si>
+    <t xml:space="preserve">requirements, tutorials, test cases, makefile, style guide, quick start
 Bibliography, quick start, README, copyright</t>
   </si>
   <si>
@@ -2251,14 +2251,14 @@
   <dimension ref="A1:AC1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="U68" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D67" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="U1" activeCellId="0" sqref="U1"/>
-      <selection pane="bottomLeft" activeCell="A68" activeCellId="0" sqref="A68"/>
-      <selection pane="bottomRight" activeCell="W73" activeCellId="0" sqref="W73"/>
+      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A67" activeCellId="0" sqref="A67"/>
+      <selection pane="bottomRight" activeCell="B73" activeCellId="0" sqref="B73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="44.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.87"/>

</xml_diff>